<commit_message>
add send email function, refactoring
</commit_message>
<xml_diff>
--- a/ozon.xlsx
+++ b/ozon.xlsx
@@ -31495,7 +31495,11 @@
           <t>Трайдекс Минск (1020000156256000)</t>
         </is>
       </c>
-      <c r="B60" s="59" t="n"/>
+      <c r="B60" s="59" t="inlineStr">
+        <is>
+          <t>0000032489</t>
+        </is>
+      </c>
       <c r="C60" s="60" t="inlineStr">
         <is>
           <t>ВО 2501 К41</t>
@@ -34003,7 +34007,11 @@
           <t>Трайдекс Минск (1020000156256000)</t>
         </is>
       </c>
-      <c r="B116" s="59" t="n"/>
+      <c r="B116" s="59" t="inlineStr">
+        <is>
+          <t>0000111724</t>
+        </is>
+      </c>
       <c r="C116" s="60" t="inlineStr">
         <is>
           <t>ПВГ 2231 К3</t>
@@ -34945,7 +34953,11 @@
           <t>Трайдекс Минск (1020000156256000)</t>
         </is>
       </c>
-      <c r="B137" s="59" t="n"/>
+      <c r="B137" s="59" t="inlineStr">
+        <is>
+          <t>0000092554</t>
+        </is>
+      </c>
       <c r="C137" s="60" t="inlineStr">
         <is>
           <t>ЭС В СН 4231</t>
@@ -34987,7 +34999,11 @@
           <t>Трайдекс Минск (1020000156256000)</t>
         </is>
       </c>
-      <c r="B138" s="59" t="n"/>
+      <c r="B138" s="59" t="inlineStr">
+        <is>
+          <t>0000215868</t>
+        </is>
+      </c>
       <c r="C138" s="60" t="inlineStr">
         <is>
           <t>ЭС В СН 4231 К43</t>
@@ -35431,7 +35447,11 @@
           <t>Трайдекс Минск (1020000156256000)</t>
         </is>
       </c>
-      <c r="B148" s="59" t="n"/>
+      <c r="B148" s="59" t="inlineStr">
+        <is>
+          <t>0000215869</t>
+        </is>
+      </c>
       <c r="C148" s="60" t="inlineStr">
         <is>
           <t>ЭС В СН 4231 К53</t>

</xml_diff>